<commit_message>
feat: get JSON data from excel worksheet
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,15 +406,1221 @@
       <c r="A1" t="str">
         <v>programName</v>
       </c>
+      <c r="B1" t="str">
+        <v>size</v>
+      </c>
+      <c r="C1" t="str">
+        <v>overallHealth</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Schedule</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Cost</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Resource</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Risk</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Comment</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Risks</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Achievements</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>CON-IT</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H2" t="str">
+        <v>string</v>
+      </c>
+      <c r="I2" t="str">
+        <v>string</v>
+      </c>
+      <c r="J2" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H3" t="str">
+        <v>string</v>
+      </c>
+      <c r="I3" t="str">
+        <v>string</v>
+      </c>
+      <c r="J3" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H4" t="str">
+        <v>string</v>
+      </c>
+      <c r="I4" t="str">
+        <v>string</v>
+      </c>
+      <c r="J4" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H5" t="str">
+        <v>string</v>
+      </c>
+      <c r="I5" t="str">
+        <v>string</v>
+      </c>
+      <c r="J5" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H6" t="str">
+        <v>string</v>
+      </c>
+      <c r="I6" t="str">
+        <v>string</v>
+      </c>
+      <c r="J6" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H7" t="str">
+        <v>string</v>
+      </c>
+      <c r="I7" t="str">
+        <v>string</v>
+      </c>
+      <c r="J7" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H8" t="str">
+        <v>string</v>
+      </c>
+      <c r="I8" t="str">
+        <v>string</v>
+      </c>
+      <c r="J8" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H9" t="str">
+        <v>string</v>
+      </c>
+      <c r="I9" t="str">
+        <v>string</v>
+      </c>
+      <c r="J9" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H10" t="str">
+        <v>string</v>
+      </c>
+      <c r="I10" t="str">
+        <v>string</v>
+      </c>
+      <c r="J10" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H11" t="str">
+        <v>string</v>
+      </c>
+      <c r="I11" t="str">
+        <v>string</v>
+      </c>
+      <c r="J11" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H12" t="str">
+        <v>string</v>
+      </c>
+      <c r="I12" t="str">
+        <v>string</v>
+      </c>
+      <c r="J12" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H13" t="str">
+        <v>string</v>
+      </c>
+      <c r="I13" t="str">
+        <v>string</v>
+      </c>
+      <c r="J13" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H14" t="str">
+        <v>string</v>
+      </c>
+      <c r="I14" t="str">
+        <v>string</v>
+      </c>
+      <c r="J14" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H15" t="str">
+        <v>string</v>
+      </c>
+      <c r="I15" t="str">
+        <v>string</v>
+      </c>
+      <c r="J15" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H16" t="str">
+        <v>string</v>
+      </c>
+      <c r="I16" t="str">
+        <v>string</v>
+      </c>
+      <c r="J16" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H17" t="str">
+        <v>string</v>
+      </c>
+      <c r="I17" t="str">
+        <v>string</v>
+      </c>
+      <c r="J17" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H18" t="str">
+        <v>string</v>
+      </c>
+      <c r="I18" t="str">
+        <v>string</v>
+      </c>
+      <c r="J18" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H19" t="str">
+        <v>string</v>
+      </c>
+      <c r="I19" t="str">
+        <v>string</v>
+      </c>
+      <c r="J19" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H20" t="str">
+        <v>string</v>
+      </c>
+      <c r="I20" t="str">
+        <v>string</v>
+      </c>
+      <c r="J20" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F21" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H21" t="str">
+        <v>string</v>
+      </c>
+      <c r="I21" t="str">
+        <v>string</v>
+      </c>
+      <c r="J21" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H22" t="str">
+        <v>string</v>
+      </c>
+      <c r="I22" t="str">
+        <v>string</v>
+      </c>
+      <c r="J22" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H23" t="str">
+        <v>string</v>
+      </c>
+      <c r="I23" t="str">
+        <v>string</v>
+      </c>
+      <c r="J23" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F24" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G24" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H24" t="str">
+        <v>string</v>
+      </c>
+      <c r="I24" t="str">
+        <v>string</v>
+      </c>
+      <c r="J24" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E25" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F25" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H25" t="str">
+        <v>string</v>
+      </c>
+      <c r="I25" t="str">
+        <v>string</v>
+      </c>
+      <c r="J25" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F26" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H26" t="str">
+        <v>string</v>
+      </c>
+      <c r="I26" t="str">
+        <v>string</v>
+      </c>
+      <c r="J26" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F27" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H27" t="str">
+        <v>string</v>
+      </c>
+      <c r="I27" t="str">
+        <v>string</v>
+      </c>
+      <c r="J27" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F28" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G28" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H28" t="str">
+        <v>string</v>
+      </c>
+      <c r="I28" t="str">
+        <v>string</v>
+      </c>
+      <c r="J28" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F29" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G29" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H29" t="str">
+        <v>string</v>
+      </c>
+      <c r="I29" t="str">
+        <v>string</v>
+      </c>
+      <c r="J29" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F30" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G30" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H30" t="str">
+        <v>string</v>
+      </c>
+      <c r="I30" t="str">
+        <v>string</v>
+      </c>
+      <c r="J30" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F31" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G31" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H31" t="str">
+        <v>string</v>
+      </c>
+      <c r="I31" t="str">
+        <v>string</v>
+      </c>
+      <c r="J31" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F32" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G32" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H32" t="str">
+        <v>string</v>
+      </c>
+      <c r="I32" t="str">
+        <v>string</v>
+      </c>
+      <c r="J32" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F33" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G33" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H33" t="str">
+        <v>string</v>
+      </c>
+      <c r="I33" t="str">
+        <v>string</v>
+      </c>
+      <c r="J33" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E34" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F34" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G34" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H34" t="str">
+        <v>string</v>
+      </c>
+      <c r="I34" t="str">
+        <v>string</v>
+      </c>
+      <c r="J34" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E35" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F35" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G35" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H35" t="str">
+        <v>string</v>
+      </c>
+      <c r="I35" t="str">
+        <v>string</v>
+      </c>
+      <c r="J35" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E36" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F36" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G36" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H36" t="str">
+        <v>string</v>
+      </c>
+      <c r="I36" t="str">
+        <v>string</v>
+      </c>
+      <c r="J36" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F37" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G37" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H37" t="str">
+        <v>string</v>
+      </c>
+      <c r="I37" t="str">
+        <v>string</v>
+      </c>
+      <c r="J37" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>CON-IT</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Green</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F38" t="str">
+        <v>Green</v>
+      </c>
+      <c r="G38" t="str">
+        <v>Green</v>
+      </c>
+      <c r="H38" t="str">
+        <v>string</v>
+      </c>
+      <c r="I38" t="str">
+        <v>string</v>
+      </c>
+      <c r="J38" t="str">
+        <v>string</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J38"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>